<commit_message>
Optimization problems & book work
Optimization problems & book work
</commit_message>
<xml_diff>
--- a/Unit_01/Unit_01_SampleWork.xlsx
+++ b/Unit_01/Unit_01_SampleWork.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\MSDS-DecisionAnalytics\Unit_01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MSDS-DecisionAnalytics\Unit_01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8185D8F-9B90-4FC9-8ABB-06AEACC3BBC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744D8A0F-C205-4A6B-9B2F-6D3418692C94}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="45540" windowHeight="23520" activeTab="6" xr2:uid="{29181C83-DE65-499E-8EBA-D0B9BD6ED8DD}"/>
+    <workbookView xWindow="-28365" yWindow="1560" windowWidth="25275" windowHeight="18105" firstSheet="3" activeTab="6" xr2:uid="{29181C83-DE65-499E-8EBA-D0B9BD6ED8DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Legos" sheetId="1" r:id="rId1"/>
@@ -20,160 +20,194 @@
     <sheet name="ThemePark" sheetId="4" r:id="rId5"/>
     <sheet name="Sensitivity Report 2" sheetId="7" r:id="rId6"/>
     <sheet name="Hot dog" sheetId="6" r:id="rId7"/>
+    <sheet name="Products" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="6" hidden="1">'Hot dog'!$C$4:$F$4</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">LegoII!$D$3:$F$3</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">LegoII3!$C$4:$H$4</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Legos!$D$3:$E$3</definedName>
+    <definedName name="solver_adj" localSheetId="7" hidden="1">Products!$D$3:$E$3</definedName>
     <definedName name="solver_adj" localSheetId="4" hidden="1">ThemePark!$C$4:$H$4</definedName>
     <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="7" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="7" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="6" hidden="1">'Hot dog'!$G$12:$G$14</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">LegoII!$G$8:$G$9</definedName>
     <definedName name="solver_lhs1" localSheetId="2" hidden="1">LegoII3!$I$9:$I$14</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Legos!$G$8:$G$9</definedName>
+    <definedName name="solver_lhs1" localSheetId="7" hidden="1">Products!$G$10</definedName>
     <definedName name="solver_lhs1" localSheetId="4" hidden="1">ThemePark!$I$9:$I$14</definedName>
     <definedName name="solver_lhs2" localSheetId="6" hidden="1">'Hot dog'!$G$9:$G$11</definedName>
+    <definedName name="solver_lhs2" localSheetId="7" hidden="1">Products!$G$8:$G$9</definedName>
     <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="7" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="7" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="7" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="7" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="6" hidden="1">'Hot dog'!$G$7</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">LegoII!$K$27</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">LegoII3!$S$6</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Legos!$H$17</definedName>
+    <definedName name="solver_opt" localSheetId="7" hidden="1">Products!$K$4</definedName>
     <definedName name="solver_opt" localSheetId="4" hidden="1">ThemePark!$I$7</definedName>
     <definedName name="solver_pre" localSheetId="6" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="7" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="6" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="7" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="6" hidden="1">'Hot dog'!$I$12:$I$14</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">LegoII!$K$8:$K$9</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">LegoII3!$K$9:$K$14</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">Legos!$K$8:$K$9</definedName>
+    <definedName name="solver_rhs1" localSheetId="7" hidden="1">Products!$K$10</definedName>
     <definedName name="solver_rhs1" localSheetId="4" hidden="1">ThemePark!$K$9:$K$14</definedName>
     <definedName name="solver_rhs2" localSheetId="6" hidden="1">'Hot dog'!$I$9:$I$11</definedName>
+    <definedName name="solver_rhs2" localSheetId="7" hidden="1">Products!$K$8:$K$9</definedName>
     <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="7" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="7" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="7" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="7" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="7" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="7" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -184,6 +218,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -191,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="114">
   <si>
     <t>Tables</t>
   </si>
@@ -515,6 +550,24 @@
   </si>
   <si>
     <t>Cholestrerol (g/lb) USED</t>
+  </si>
+  <si>
+    <t>Working Hours</t>
+  </si>
+  <si>
+    <t>Machine Hours</t>
+  </si>
+  <si>
+    <t>Product 1</t>
+  </si>
+  <si>
+    <t>Product 2</t>
+  </si>
+  <si>
+    <t>&gt;=</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -523,9 +576,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1264,58 +1317,22 @@
   <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1325,9 +1342,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1337,9 +1351,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1377,28 +1388,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="30" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1408,12 +1398,6 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1422,9 +1406,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1433,21 +1414,15 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="11" fillId="6" borderId="14" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="14" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="7" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="7" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1456,9 +1431,6 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1509,8 +1481,89 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="18" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="11" fillId="8" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="11" fillId="8" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="30" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2177,7 +2230,7 @@
   <dimension ref="A2:L9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+      <selection activeCell="K14" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2199,10 +2252,10 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>3</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>6</v>
       </c>
       <c r="K3" t="s">
@@ -2219,11 +2272,11 @@
       <c r="E4">
         <v>10</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="71">
         <f>SUMPRODUCT(D4:E4,D3:E3)</f>
         <v>108</v>
       </c>
-      <c r="L4" s="3"/>
+      <c r="L4" s="72"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G5" s="1" t="s">
@@ -2319,7 +2372,7 @@
   <dimension ref="A2:L9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2344,13 +2397,13 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>8</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <v>2</v>
       </c>
       <c r="K3" t="s">
@@ -2370,11 +2423,11 @@
       <c r="F4">
         <v>15</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="71">
         <f>SUMPRODUCT(D4:F4,D3:F3)</f>
         <v>110</v>
       </c>
-      <c r="L4" s="3"/>
+      <c r="L4" s="72"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G5" s="1" t="s">
@@ -2504,13 +2557,13 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>8</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <v>2</v>
       </c>
       <c r="K3" t="s">
@@ -2530,11 +2583,11 @@
       <c r="F4">
         <v>13.5</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="71">
         <f>SUMPRODUCT(D4:F4,D3:F3)</f>
         <v>99</v>
       </c>
-      <c r="L4" s="3"/>
+      <c r="L4" s="72"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G5" s="1" t="s">
@@ -2654,17 +2707,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="29" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="29" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2674,182 +2727,182 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46" t="s">
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="46" t="s">
+      <c r="F7" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="46" t="s">
+      <c r="G7" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="46" t="s">
+      <c r="H7" s="32" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="47" t="s">
+      <c r="E8" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="47" t="s">
+      <c r="F8" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="47" t="s">
+      <c r="G8" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="33" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="44">
+      <c r="D9" s="30">
         <v>90</v>
       </c>
-      <c r="E9" s="44">
+      <c r="E9" s="30">
         <v>0</v>
       </c>
-      <c r="F9" s="44">
-        <v>1</v>
-      </c>
-      <c r="G9" s="44">
+      <c r="F9" s="30">
+        <v>1</v>
+      </c>
+      <c r="G9" s="30">
         <v>0</v>
       </c>
-      <c r="H9" s="44">
+      <c r="H9" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="30">
         <v>125</v>
       </c>
-      <c r="E10" s="44">
+      <c r="E10" s="30">
         <v>0</v>
       </c>
-      <c r="F10" s="44">
-        <v>1</v>
-      </c>
-      <c r="G10" s="44">
-        <v>1</v>
-      </c>
-      <c r="H10" s="44">
+      <c r="F10" s="30">
+        <v>1</v>
+      </c>
+      <c r="G10" s="30">
+        <v>1</v>
+      </c>
+      <c r="H10" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="44">
+      <c r="D11" s="30">
         <v>125</v>
       </c>
-      <c r="E11" s="44">
+      <c r="E11" s="30">
         <v>0</v>
       </c>
-      <c r="F11" s="44">
-        <v>1</v>
-      </c>
-      <c r="G11" s="44">
+      <c r="F11" s="30">
+        <v>1</v>
+      </c>
+      <c r="G11" s="30">
         <v>0</v>
       </c>
-      <c r="H11" s="44">
+      <c r="H11" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="44">
+      <c r="D12" s="30">
         <v>175</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="30">
         <v>0</v>
       </c>
-      <c r="F12" s="44">
-        <v>1</v>
-      </c>
-      <c r="G12" s="44">
+      <c r="F12" s="30">
+        <v>1</v>
+      </c>
+      <c r="G12" s="30">
         <v>0</v>
       </c>
-      <c r="H12" s="44">
+      <c r="H12" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="44">
+      <c r="D13" s="30">
         <v>125</v>
       </c>
-      <c r="E13" s="44">
+      <c r="E13" s="30">
         <v>0</v>
       </c>
-      <c r="F13" s="44">
-        <v>1</v>
-      </c>
-      <c r="G13" s="44">
+      <c r="F13" s="30">
+        <v>1</v>
+      </c>
+      <c r="G13" s="30">
         <v>0</v>
       </c>
-      <c r="H13" s="44">
+      <c r="H13" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="45">
+      <c r="D14" s="31">
         <v>0</v>
       </c>
-      <c r="E14" s="45">
+      <c r="E14" s="31">
         <v>0</v>
       </c>
-      <c r="F14" s="45">
-        <v>1</v>
-      </c>
-      <c r="G14" s="45">
+      <c r="F14" s="31">
+        <v>1</v>
+      </c>
+      <c r="G14" s="31">
         <v>1E+30</v>
       </c>
-      <c r="H14" s="45">
+      <c r="H14" s="31">
         <v>0</v>
       </c>
     </row>
@@ -2859,182 +2912,182 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46" t="s">
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="46" t="s">
+      <c r="E17" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="46" t="s">
+      <c r="F17" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="46" t="s">
+      <c r="G17" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="46" t="s">
+      <c r="H17" s="32" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="D18" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="47" t="s">
+      <c r="E18" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="47" t="s">
+      <c r="F18" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="47" t="s">
+      <c r="G18" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="47" t="s">
+      <c r="H18" s="33" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="44">
+      <c r="D19" s="30">
         <v>90</v>
       </c>
-      <c r="E19" s="44">
-        <v>1</v>
-      </c>
-      <c r="F19" s="44">
+      <c r="E19" s="30">
+        <v>1</v>
+      </c>
+      <c r="F19" s="30">
         <v>90</v>
       </c>
-      <c r="G19" s="44">
+      <c r="G19" s="30">
         <v>125</v>
       </c>
-      <c r="H19" s="44">
+      <c r="H19" s="30">
         <v>90</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="44">
+      <c r="D20" s="30">
         <v>215</v>
       </c>
-      <c r="E20" s="44">
+      <c r="E20" s="30">
         <v>0</v>
       </c>
-      <c r="F20" s="44">
+      <c r="F20" s="30">
         <v>215</v>
       </c>
-      <c r="G20" s="44">
+      <c r="G20" s="30">
         <v>125</v>
       </c>
-      <c r="H20" s="44">
+      <c r="H20" s="30">
         <v>125</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="44" t="s">
+      <c r="C21" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="44">
+      <c r="D21" s="30">
         <v>250</v>
       </c>
-      <c r="E21" s="44">
-        <v>1</v>
-      </c>
-      <c r="F21" s="44">
+      <c r="E21" s="30">
+        <v>1</v>
+      </c>
+      <c r="F21" s="30">
         <v>250</v>
       </c>
-      <c r="G21" s="44">
+      <c r="G21" s="30">
         <v>1E+30</v>
       </c>
-      <c r="H21" s="44">
+      <c r="H21" s="30">
         <v>125</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="44" t="s">
+      <c r="C22" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="44">
+      <c r="D22" s="30">
         <v>300</v>
       </c>
-      <c r="E22" s="44">
+      <c r="E22" s="30">
         <v>0</v>
       </c>
-      <c r="F22" s="44">
+      <c r="F22" s="30">
         <v>165</v>
       </c>
-      <c r="G22" s="44">
+      <c r="G22" s="30">
         <v>135</v>
       </c>
-      <c r="H22" s="44">
+      <c r="H22" s="30">
         <v>1E+30</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="44">
+      <c r="D23" s="30">
         <v>300</v>
       </c>
-      <c r="E23" s="44">
-        <v>1</v>
-      </c>
-      <c r="F23" s="44">
+      <c r="E23" s="30">
+        <v>1</v>
+      </c>
+      <c r="F23" s="30">
         <v>300</v>
       </c>
-      <c r="G23" s="44">
+      <c r="G23" s="30">
         <v>1E+30</v>
       </c>
-      <c r="H23" s="44">
+      <c r="H23" s="30">
         <v>135</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="45" t="s">
+      <c r="B24" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="45" t="s">
+      <c r="C24" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="45">
+      <c r="D24" s="31">
         <v>125</v>
       </c>
-      <c r="E24" s="45">
+      <c r="E24" s="31">
         <v>0</v>
       </c>
-      <c r="F24" s="45">
+      <c r="F24" s="31">
         <v>125</v>
       </c>
-      <c r="G24" s="45">
+      <c r="G24" s="31">
         <v>135</v>
       </c>
-      <c r="H24" s="45">
+      <c r="H24" s="31">
         <v>125</v>
       </c>
     </row>
@@ -3054,316 +3107,316 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="9" style="5"/>
-    <col min="9" max="9" width="11.140625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="9" style="5"/>
-    <col min="11" max="11" width="7.7109375" style="5" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="5"/>
+    <col min="1" max="1" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="9" style="3"/>
+    <col min="9" max="9" width="11.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9" style="3"/>
+    <col min="11" max="11" width="7.7109375" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="6"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="12" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="74"/>
+      <c r="C2" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="80"/>
     </row>
     <row r="3" spans="1:11" ht="12" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13" t="s">
+      <c r="A3" s="75"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="12" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16">
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="6">
         <v>90</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="6">
         <v>125</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="6">
         <v>125</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="6">
         <v>175</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="6">
         <v>125</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="11.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="20" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="22" t="s">
+      <c r="A7" s="82"/>
+      <c r="B7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="23">
-        <v>1</v>
-      </c>
-      <c r="D7" s="23">
-        <v>1</v>
-      </c>
-      <c r="E7" s="23">
-        <v>1</v>
-      </c>
-      <c r="F7" s="23">
-        <v>1</v>
-      </c>
-      <c r="G7" s="23">
-        <v>1</v>
-      </c>
-      <c r="H7" s="23">
-        <v>1</v>
-      </c>
-      <c r="I7" s="24">
+      <c r="C7" s="11">
+        <v>1</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1</v>
+      </c>
+      <c r="E7" s="11">
+        <v>1</v>
+      </c>
+      <c r="F7" s="11">
+        <v>1</v>
+      </c>
+      <c r="G7" s="11">
+        <v>1</v>
+      </c>
+      <c r="H7" s="11">
+        <v>1</v>
+      </c>
+      <c r="I7" s="12">
         <f>SUMPRODUCT(C7:H7,C$4:H$4)</f>
         <v>640</v>
       </c>
-      <c r="J7" s="25"/>
+      <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:11" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="J8" s="26"/>
+      <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="29">
-        <v>1</v>
-      </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29">
-        <v>1</v>
-      </c>
-      <c r="I9" s="30">
+      <c r="C9" s="16">
+        <v>1</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16">
+        <v>1</v>
+      </c>
+      <c r="I9" s="17">
         <f>SUMPRODUCT(C9:H9,C$4:H$4)</f>
         <v>90</v>
       </c>
-      <c r="J9" s="42" t="s">
+      <c r="J9" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="K9" s="31">
+      <c r="K9" s="18">
         <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
-      <c r="B10" s="33" t="s">
+      <c r="A10" s="84"/>
+      <c r="B10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="34">
-        <v>1</v>
-      </c>
-      <c r="D10" s="34">
-        <v>1</v>
-      </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="30">
+      <c r="C10" s="20">
+        <v>1</v>
+      </c>
+      <c r="D10" s="20">
+        <v>1</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="17">
         <f t="shared" ref="I10:I14" si="0">SUMPRODUCT(C10:H10,C$4:H$4)</f>
         <v>215</v>
       </c>
-      <c r="J10" s="42" t="s">
+      <c r="J10" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="35">
+      <c r="K10" s="21">
         <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="32"/>
-      <c r="B11" s="33" t="s">
+      <c r="A11" s="84"/>
+      <c r="B11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34">
-        <v>1</v>
-      </c>
-      <c r="E11" s="34">
-        <v>1</v>
-      </c>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="30">
+      <c r="C11" s="20"/>
+      <c r="D11" s="20">
+        <v>1</v>
+      </c>
+      <c r="E11" s="20">
+        <v>1</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="17">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="J11" s="42" t="s">
+      <c r="J11" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="K11" s="35">
+      <c r="K11" s="21">
         <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33" t="s">
+      <c r="A12" s="84"/>
+      <c r="B12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34">
-        <v>1</v>
-      </c>
-      <c r="F12" s="34">
-        <v>1</v>
-      </c>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="30">
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20">
+        <v>1</v>
+      </c>
+      <c r="F12" s="20">
+        <v>1</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="17">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="J12" s="42" t="s">
+      <c r="J12" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="35">
+      <c r="K12" s="21">
         <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33" t="s">
+      <c r="A13" s="84"/>
+      <c r="B13" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34">
-        <v>1</v>
-      </c>
-      <c r="G13" s="34">
-        <v>1</v>
-      </c>
-      <c r="H13" s="34"/>
-      <c r="I13" s="30">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20">
+        <v>1</v>
+      </c>
+      <c r="G13" s="20">
+        <v>1</v>
+      </c>
+      <c r="H13" s="20"/>
+      <c r="I13" s="17">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="J13" s="42" t="s">
+      <c r="J13" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="K13" s="35">
+      <c r="K13" s="21">
         <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
-      <c r="B14" s="33" t="s">
+      <c r="A14" s="84"/>
+      <c r="B14" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34">
-        <v>1</v>
-      </c>
-      <c r="H14" s="34">
-        <v>1</v>
-      </c>
-      <c r="I14" s="30">
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20">
+        <v>1</v>
+      </c>
+      <c r="H14" s="20">
+        <v>1</v>
+      </c>
+      <c r="I14" s="17">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="J14" s="42" t="s">
+      <c r="J14" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="K14" s="35">
+      <c r="K14" s="21">
         <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="36"/>
-      <c r="B15" s="37" t="s">
+      <c r="A15" s="22"/>
+      <c r="B15" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="40"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="26"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3396,17 +3449,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="29" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="29" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="29" t="s">
         <v>95</v>
       </c>
     </row>
@@ -3416,136 +3469,136 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46" t="s">
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="46" t="s">
+      <c r="F7" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="46" t="s">
+      <c r="G7" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="46" t="s">
+      <c r="H7" s="32" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="47" t="s">
+      <c r="E8" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="47" t="s">
+      <c r="F8" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="47" t="s">
+      <c r="G8" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="47" t="s">
+      <c r="H8" s="33" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="44">
+      <c r="D9" s="30">
         <v>8.8378527946873259E-2</v>
       </c>
-      <c r="E9" s="44">
+      <c r="E9" s="30">
         <v>0</v>
       </c>
-      <c r="F9" s="44">
+      <c r="F9" s="30">
         <v>0.76</v>
       </c>
-      <c r="G9" s="44">
+      <c r="G9" s="30">
         <v>8.0000000000000168E-2</v>
       </c>
-      <c r="H9" s="44">
+      <c r="H9" s="30">
         <v>5.3266866976235804E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="30">
         <v>4.1173215273934707E-2</v>
       </c>
-      <c r="E10" s="44">
+      <c r="E10" s="30">
         <v>0</v>
       </c>
-      <c r="F10" s="44">
+      <c r="F10" s="30">
         <v>0.82000000000000006</v>
       </c>
-      <c r="G10" s="44">
+      <c r="G10" s="30">
         <v>0.43281249999999977</v>
       </c>
-      <c r="H10" s="44">
+      <c r="H10" s="30">
         <v>7.8095238095238245E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="44">
+      <c r="D11" s="30">
         <v>0</v>
       </c>
-      <c r="E11" s="44">
+      <c r="E11" s="30">
         <v>-0.17607083563918077</v>
       </c>
-      <c r="F11" s="44">
+      <c r="F11" s="30">
         <v>0.64000000000000012</v>
       </c>
-      <c r="G11" s="44">
+      <c r="G11" s="30">
         <v>0.17607083563918077</v>
       </c>
-      <c r="H11" s="44">
+      <c r="H11" s="30">
         <v>1E+30</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="45">
+      <c r="D12" s="31">
         <v>0</v>
       </c>
-      <c r="E12" s="45">
+      <c r="E12" s="31">
         <v>-4.3167681239623522E-2</v>
       </c>
-      <c r="F12" s="45">
+      <c r="F12" s="31">
         <v>0.58000000000000007</v>
       </c>
-      <c r="G12" s="45">
+      <c r="G12" s="31">
         <v>4.3167681239623522E-2</v>
       </c>
-      <c r="H12" s="45">
+      <c r="H12" s="31">
         <v>1E+30</v>
       </c>
     </row>
@@ -3555,182 +3608,182 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46" t="s">
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="46" t="s">
+      <c r="E15" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="46" t="s">
+      <c r="F15" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="46" t="s">
+      <c r="G15" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="46" t="s">
+      <c r="H15" s="32" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="47" t="s">
+      <c r="D16" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="47" t="s">
+      <c r="E16" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="47" t="s">
+      <c r="F16" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="G16" s="47" t="s">
+      <c r="G16" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="33" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D17" s="44">
+      <c r="D17" s="30">
         <v>8.8378527946873259E-2</v>
       </c>
-      <c r="E17" s="44">
+      <c r="E17" s="30">
         <v>0</v>
       </c>
-      <c r="F17" s="44">
+      <c r="F17" s="30">
         <v>0</v>
       </c>
-      <c r="G17" s="44">
+      <c r="G17" s="30">
         <v>6.6283895960154951E-2</v>
       </c>
-      <c r="H17" s="44">
+      <c r="H17" s="30">
         <v>1E+30</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="D18" s="44">
+      <c r="D18" s="30">
         <v>4.1173215273934707E-2</v>
       </c>
-      <c r="E18" s="44">
+      <c r="E18" s="30">
         <v>0</v>
       </c>
-      <c r="F18" s="44">
+      <c r="F18" s="30">
         <v>0</v>
       </c>
-      <c r="G18" s="44">
+      <c r="G18" s="30">
         <v>3.0879911455451031E-2</v>
       </c>
-      <c r="H18" s="44">
+      <c r="H18" s="30">
         <v>1E+30</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="D19" s="44">
+      <c r="D19" s="30">
         <v>0.12955174322080798</v>
       </c>
-      <c r="E19" s="44">
+      <c r="E19" s="30">
         <v>0</v>
       </c>
-      <c r="F19" s="44">
+      <c r="F19" s="30">
         <v>0</v>
       </c>
-      <c r="G19" s="44">
+      <c r="G19" s="30">
         <v>4.5517432208079696E-3</v>
       </c>
-      <c r="H19" s="44">
+      <c r="H19" s="30">
         <v>1E+30</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="D20" s="44">
+      <c r="D20" s="30">
         <v>100</v>
       </c>
-      <c r="E20" s="44">
+      <c r="E20" s="30">
         <v>1.8151632540121785E-4</v>
       </c>
-      <c r="F20" s="44">
+      <c r="F20" s="30">
         <v>100</v>
       </c>
-      <c r="G20" s="44">
+      <c r="G20" s="30">
         <v>17.4681988241582</v>
       </c>
-      <c r="H20" s="44">
+      <c r="H20" s="30">
         <v>17.714285714285715</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="44" t="s">
+      <c r="C21" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="D21" s="44">
+      <c r="D21" s="30">
         <v>5.0956557830658546</v>
       </c>
-      <c r="E21" s="44">
+      <c r="E21" s="30">
         <v>0</v>
       </c>
-      <c r="F21" s="44">
+      <c r="F21" s="30">
         <v>6</v>
       </c>
-      <c r="G21" s="44">
+      <c r="G21" s="30">
         <v>1E+30</v>
       </c>
-      <c r="H21" s="44">
+      <c r="H21" s="30">
         <v>0.9043442169341448</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="45" t="s">
+      <c r="C22" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="45">
+      <c r="D22" s="31">
         <v>27</v>
       </c>
-      <c r="E22" s="45">
+      <c r="E22" s="31">
         <v>3.0658550083010501E-3</v>
       </c>
-      <c r="F22" s="45">
+      <c r="F22" s="31">
         <v>27</v>
       </c>
-      <c r="G22" s="45">
+      <c r="G22" s="31">
         <v>5.8125</v>
       </c>
-      <c r="H22" s="45">
+      <c r="H22" s="31">
         <v>0.99096385542168686</v>
       </c>
     </row>
@@ -3745,442 +3798,442 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+      <selection activeCell="C9" sqref="C9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9" style="5"/>
-    <col min="7" max="7" width="10.42578125" style="5" customWidth="1"/>
-    <col min="8" max="9" width="9" style="5"/>
-    <col min="10" max="10" width="7.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="5"/>
+    <col min="1" max="1" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9" style="3"/>
+    <col min="7" max="7" width="10.42578125" style="3" customWidth="1"/>
+    <col min="8" max="9" width="9" style="3"/>
+    <col min="10" max="10" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="48"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="51" t="s">
+      <c r="B2" s="86"/>
+      <c r="C2" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="54"/>
-      <c r="J2" s="48"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="35"/>
+      <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A3" s="55"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="57" t="s">
+      <c r="A3" s="87"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="G3" s="54"/>
-      <c r="J3" s="48"/>
+      <c r="G3" s="35"/>
+      <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:12" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="60"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="62">
+      <c r="A4" s="89"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="39">
         <v>3.125E-2</v>
       </c>
-      <c r="D4" s="63">
+      <c r="D4" s="40">
         <v>3.125E-2</v>
       </c>
-      <c r="E4" s="63">
+      <c r="E4" s="40">
         <v>0</v>
       </c>
-      <c r="F4" s="63">
+      <c r="F4" s="40">
         <v>6.25E-2</v>
       </c>
-      <c r="G4" s="64"/>
-      <c r="J4" s="48"/>
+      <c r="G4" s="41"/>
+      <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:12" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="54"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="J5" s="48"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="J5" s="34"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="68" t="s">
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="48"/>
+      <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:12" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="69"/>
-      <c r="B7" s="70" t="s">
+      <c r="A7" s="95"/>
+      <c r="B7" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="71">
+      <c r="C7" s="46">
         <v>0.76</v>
       </c>
-      <c r="D7" s="71">
+      <c r="D7" s="46">
         <v>0.82</v>
       </c>
-      <c r="E7" s="71">
+      <c r="E7" s="46">
         <v>0.64</v>
       </c>
-      <c r="F7" s="71">
+      <c r="F7" s="46">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G7" s="72">
+      <c r="G7" s="47">
         <f>SUMPRODUCT(C7:F7,C4:F4)</f>
         <v>8.5625000000000007E-2</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="J7" s="48"/>
+      <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:12" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="73" t="s">
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="I8" s="48" t="s">
+      <c r="I8" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="J8" s="48"/>
+      <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:12" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="74" t="s">
+      <c r="A9" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="76">
+      <c r="C9" s="50">
         <v>640</v>
       </c>
-      <c r="D9" s="76">
+      <c r="D9" s="50">
         <v>1055</v>
       </c>
-      <c r="E9" s="76">
+      <c r="E9" s="50">
         <v>780</v>
       </c>
-      <c r="F9" s="76">
+      <c r="F9" s="50">
         <v>528</v>
       </c>
-      <c r="G9" s="97">
+      <c r="G9" s="70">
         <f>SUMPRODUCT(C9:F9,C$4:F$4)</f>
         <v>85.96875</v>
       </c>
-      <c r="H9" s="77" t="s">
+      <c r="H9" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="18">
         <v>100</v>
       </c>
-      <c r="J9" s="48" t="s">
+      <c r="J9" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
     </row>
     <row r="10" spans="1:12" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="78"/>
-      <c r="B10" s="79" t="s">
+      <c r="A10" s="97"/>
+      <c r="B10" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="76">
+      <c r="C10" s="50">
         <v>32.5</v>
       </c>
-      <c r="D10" s="76">
+      <c r="D10" s="50">
         <v>54</v>
       </c>
-      <c r="E10" s="76">
+      <c r="E10" s="50">
         <v>25.6</v>
       </c>
-      <c r="F10" s="76">
+      <c r="F10" s="50">
         <v>6.4</v>
       </c>
-      <c r="G10" s="97">
+      <c r="G10" s="70">
         <f t="shared" ref="G10:G14" si="0">SUMPRODUCT(C10:F10,C$4:F$4)</f>
         <v>3.1031249999999999</v>
       </c>
-      <c r="H10" s="77" t="s">
+      <c r="H10" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="35">
+      <c r="I10" s="21">
         <v>6</v>
       </c>
-      <c r="J10" s="48" t="s">
+      <c r="J10" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
     </row>
     <row r="11" spans="1:12" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="78"/>
-      <c r="B11" s="79" t="s">
+      <c r="A11" s="97"/>
+      <c r="B11" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="76">
+      <c r="C11" s="50">
         <v>210</v>
       </c>
-      <c r="D11" s="76">
+      <c r="D11" s="50">
         <v>205</v>
       </c>
-      <c r="E11" s="76">
+      <c r="E11" s="50">
         <v>220</v>
       </c>
-      <c r="F11" s="76">
+      <c r="F11" s="50">
         <v>172</v>
       </c>
-      <c r="G11" s="97">
+      <c r="G11" s="70">
         <f t="shared" si="0"/>
         <v>23.71875</v>
       </c>
-      <c r="H11" s="77" t="s">
+      <c r="H11" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="35">
+      <c r="I11" s="21">
         <v>27</v>
       </c>
-      <c r="J11" s="48" t="s">
+      <c r="J11" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
     </row>
     <row r="12" spans="1:12" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="78"/>
-      <c r="B12" s="79" t="s">
+      <c r="A12" s="97"/>
+      <c r="B12" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="76">
-        <v>1</v>
-      </c>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="97">
+      <c r="C12" s="50">
+        <v>1</v>
+      </c>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="70">
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
-      <c r="H12" s="96" t="s">
+      <c r="H12" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="35">
+      <c r="I12" s="21">
         <f>J12*I14</f>
         <v>3.125E-2</v>
       </c>
-      <c r="J12" s="80">
+      <c r="J12" s="53">
         <v>0.25</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="78"/>
-      <c r="B13" s="79" t="s">
+      <c r="A13" s="97"/>
+      <c r="B13" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76">
-        <v>1</v>
-      </c>
-      <c r="E13" s="76"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="97">
+      <c r="C13" s="50"/>
+      <c r="D13" s="50">
+        <v>1</v>
+      </c>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="70">
         <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
-      <c r="H13" s="96" t="s">
+      <c r="H13" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="I13" s="35">
+      <c r="I13" s="21">
         <f>I14*J13</f>
         <v>3.125E-2</v>
       </c>
-      <c r="J13" s="80">
+      <c r="J13" s="53">
         <v>0.25</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="76">
-        <v>1</v>
-      </c>
-      <c r="D14" s="76">
-        <v>1</v>
-      </c>
-      <c r="E14" s="76">
-        <v>1</v>
-      </c>
-      <c r="F14" s="76">
-        <v>1</v>
-      </c>
-      <c r="G14" s="97">
+      <c r="C14" s="50">
+        <v>1</v>
+      </c>
+      <c r="D14" s="50">
+        <v>1</v>
+      </c>
+      <c r="E14" s="50">
+        <v>1</v>
+      </c>
+      <c r="F14" s="50">
+        <v>1</v>
+      </c>
+      <c r="G14" s="70">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="H14" s="96" t="s">
+      <c r="H14" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="82">
+      <c r="I14" s="55">
         <f>K14/16</f>
         <v>0.125</v>
       </c>
-      <c r="J14" s="48" t="s">
+      <c r="J14" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="K14" s="83">
+      <c r="K14" s="56">
         <v>2</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="L14" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="G15" s="48"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="48"/>
+      <c r="G15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
     </row>
     <row r="16" spans="1:12" ht="11.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="84" t="s">
+      <c r="C16" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="85" t="s">
+      <c r="D16" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="85" t="s">
+      <c r="E16" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="86" t="s">
+      <c r="F16" s="59" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="88">
+      <c r="C17" s="61">
         <v>0.76</v>
       </c>
-      <c r="D17" s="88">
+      <c r="D17" s="61">
         <v>0.82</v>
       </c>
-      <c r="E17" s="88">
+      <c r="E17" s="61">
         <v>0.64</v>
       </c>
-      <c r="F17" s="89">
+      <c r="F17" s="62">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G17" s="90" t="s">
+      <c r="G17" s="63" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="B18" s="91" t="s">
+      <c r="B18" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="92">
+      <c r="C18" s="65">
         <v>640</v>
       </c>
-      <c r="D18" s="92">
+      <c r="D18" s="65">
         <v>1055</v>
       </c>
-      <c r="E18" s="92">
+      <c r="E18" s="65">
         <v>780</v>
       </c>
-      <c r="F18" s="92">
+      <c r="F18" s="65">
         <v>528</v>
       </c>
-      <c r="G18" s="93">
+      <c r="G18" s="66">
         <v>100</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="95">
+      <c r="C19" s="68">
         <v>32.5</v>
       </c>
-      <c r="D19" s="95">
+      <c r="D19" s="68">
         <v>54</v>
       </c>
-      <c r="E19" s="95">
+      <c r="E19" s="68">
         <v>25.6</v>
       </c>
-      <c r="F19" s="95">
+      <c r="F19" s="68">
         <v>6.4</v>
       </c>
-      <c r="G19" s="93">
+      <c r="G19" s="66">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="B20" s="94" t="s">
+      <c r="B20" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="95">
+      <c r="C20" s="68">
         <v>210</v>
       </c>
-      <c r="D20" s="95">
+      <c r="D20" s="68">
         <v>205</v>
       </c>
-      <c r="E20" s="95">
+      <c r="E20" s="68">
         <v>220</v>
       </c>
-      <c r="F20" s="95">
+      <c r="F20" s="68">
         <v>172</v>
       </c>
-      <c r="G20" s="93">
+      <c r="G20" s="66">
         <v>27</v>
       </c>
     </row>
@@ -4194,4 +4247,167 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECBF69D-DDB4-499D-A42D-95AEAC76F832}">
+  <dimension ref="A2:L10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>19.999999999999996</v>
+      </c>
+      <c r="E3" s="2">
+        <v>75</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>60</v>
+      </c>
+      <c r="K4" s="71">
+        <f>SUMPRODUCT(D4:E4,D3:E3)</f>
+        <v>4900</v>
+      </c>
+      <c r="L4" s="72"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8">
+        <v>30</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="G8" s="1">
+        <f>SUMPRODUCT(D8:E8,$D$3:$E$3)</f>
+        <v>2100</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1">
+        <f>SUMPRODUCT(D9:E9,$D$3:$E$3)</f>
+        <v>850</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <f>SUMPRODUCT(D10:E10,D3:E3)</f>
+        <v>95</v>
+      </c>
+      <c r="J10" t="s">
+        <v>112</v>
+      </c>
+      <c r="K10">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K4:L4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>